<commit_message>
EcommerceFront - Modulo - En Construccion v1
</commit_message>
<xml_diff>
--- a/Documentacion/Base de Datos CBD v1.xlsx
+++ b/Documentacion/Base de Datos CBD v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oavalos/Documents/Personal/Proyecto CBD/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EED531-4B06-E545-AD53-C587D3C3EEE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA4F1CB-5A56-4C47-B266-2BDFC6004B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{D4FEB497-8318-AB43-A3DA-832786BD3E10}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{D4FEB497-8318-AB43-A3DA-832786BD3E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Estructura" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="143">
   <si>
     <t>nombre</t>
   </si>
@@ -196,9 +196,6 @@
     <t>id_tipo_cliente</t>
   </si>
   <si>
-    <t>identificacion_tipo</t>
-  </si>
-  <si>
     <t>identificacion_numero</t>
   </si>
   <si>
@@ -316,9 +313,6 @@
     <t>Pendiente, Enviado, Cancelado, Etc.</t>
   </si>
   <si>
-    <t>Tabla: cbd_direcciones _entrega</t>
-  </si>
-  <si>
     <t>cve_direccion_entrega</t>
   </si>
   <si>
@@ -349,9 +343,6 @@
     <t>cve_pedido_estatus</t>
   </si>
   <si>
-    <t>Tabla: cbd_direcciones _facturacion</t>
-  </si>
-  <si>
     <t>cve_direccion_facturacion</t>
   </si>
   <si>
@@ -455,6 +446,15 @@
   </si>
   <si>
     <t>ruta_miniatura</t>
+  </si>
+  <si>
+    <t>Tabla: cbd_direcciones_entrega</t>
+  </si>
+  <si>
+    <t>Tabla: cbd_direcciones_facturacion</t>
+  </si>
+  <si>
+    <t>id_tipo_identificacion</t>
   </si>
 </sst>
 </file>
@@ -1030,6 +1030,54 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1048,15 +1096,6 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1066,15 +1105,6 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1111,46 +1141,16 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1339,16 +1339,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>2616200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1382889</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>112889</xdr:rowOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1362,119 +1362,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9479844" y="5954889"/>
-          <a:ext cx="2937934" cy="1227667"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 32879"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1968500</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>98778</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1382889</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="33" name="Conector angular 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5335C99C-17E2-3443-876E-9910CB9B3A1A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7838722" y="7775222"/>
-          <a:ext cx="4579056" cy="1044222"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 57011"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>112889</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="34" name="Conector angular 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7900404-9446-D847-BF1A-87099EDD57AC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="9454444" y="7380111"/>
-          <a:ext cx="2991556" cy="1411"/>
+          <a:off x="9740900" y="7656689"/>
+          <a:ext cx="3922889" cy="3532011"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -1504,16 +1394,126 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1968500</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1435100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>98778</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1382889</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Conector angular 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5335C99C-17E2-3443-876E-9910CB9B3A1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4940300" y="8252178"/>
+          <a:ext cx="8723489" cy="5882922"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 87997"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>112889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Conector angular 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7900404-9446-D847-BF1A-87099EDD57AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5105400" y="7859889"/>
+          <a:ext cx="8585200" cy="4814711"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 83580"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>98778</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1397000</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1528,12 +1528,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="7838722" y="7986889"/>
-          <a:ext cx="4593167" cy="2455333"/>
+          <a:off x="4724400" y="8455378"/>
+          <a:ext cx="8953500" cy="7356122"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 70002"/>
+            <a:gd name="adj1" fmla="val 92270"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1724,116 +1724,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1915948</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>112889</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1382889</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>98535</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="69" name="Conector angular 68">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DC646EC-FC9D-B446-A45B-4488B627BBB5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7786170" y="8198556"/>
-          <a:ext cx="4631608" cy="3640423"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 80214"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1490134</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>98778</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>1368778</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="82" name="Conector angular 81">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{473F092B-E0FD-294C-85E4-30414056E697}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3747912" y="8396111"/>
-          <a:ext cx="8655755" cy="7636933"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 94370"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>1965739</xdr:colOff>
       <xdr:row>39</xdr:row>
@@ -1944,61 +1834,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>22579</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>804334</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="113" name="Conector angular 112">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D054B400-FAFB-2B4A-8B4B-B6595EB79495}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10740821" y="7928429"/>
-          <a:ext cx="13663183" cy="9039748"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 94000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>56</xdr:row>
@@ -2029,6 +1864,116 @@
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
             <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1308100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1384300</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector angular 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A47FAF0-464F-6B4C-839B-4D16B627C3D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="8432800" y="6007100"/>
+          <a:ext cx="5232400" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 15777"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="31" name="Conector angular 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9F19A80-E81B-2546-B097-FC1C1277CC17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="8521700" y="1422400"/>
+          <a:ext cx="5130800" cy="4533900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 16089"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2352,9 +2297,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770F6DCC-4CB2-7A4E-A798-91BAB4EC9683}">
-  <dimension ref="A1:AM96"/>
+  <dimension ref="A1:AM81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2409,24 +2356,89 @@
       <c r="I1" s="65"/>
       <c r="J1" s="65"/>
     </row>
-    <row r="5" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C3" s="135" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="136"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="136"/>
+      <c r="G3" s="137"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C4" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="101" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="102" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="98" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="99" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="99" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="99" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="11"/>
+    </row>
     <row r="6" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K6" s="150" t="s">
+      <c r="C6" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="K6" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="151"/>
-      <c r="M6" s="151"/>
-      <c r="N6" s="151"/>
-      <c r="O6" s="152"/>
-      <c r="S6" s="128" t="s">
+      <c r="L6" s="117"/>
+      <c r="M6" s="117"/>
+      <c r="N6" s="117"/>
+      <c r="O6" s="118"/>
+      <c r="S6" s="119" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="153"/>
-      <c r="W6" s="130"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="120"/>
+      <c r="V6" s="121"/>
+      <c r="W6" s="122"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C7" s="25"/>
+      <c r="D7" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="5"/>
       <c r="K7" s="27" t="s">
         <v>22</v>
       </c>
@@ -2457,15 +2469,26 @@
       <c r="W7" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="AI7" s="128" t="s">
-        <v>119</v>
-      </c>
-      <c r="AJ7" s="129"/>
-      <c r="AK7" s="129"/>
-      <c r="AL7" s="129"/>
-      <c r="AM7" s="130"/>
+      <c r="AI7" s="119" t="s">
+        <v>116</v>
+      </c>
+      <c r="AJ7" s="120"/>
+      <c r="AK7" s="120"/>
+      <c r="AL7" s="120"/>
+      <c r="AM7" s="122"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C8" s="25"/>
+      <c r="D8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="5"/>
       <c r="K8" s="24" t="s">
         <v>23</v>
       </c>
@@ -2509,6 +2532,17 @@
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C9" s="25"/>
+      <c r="D9" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="K9" s="25"/>
       <c r="L9" s="19" t="s">
         <v>18</v>
@@ -2539,7 +2573,7 @@
         <v>23</v>
       </c>
       <c r="AJ9" s="38" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="AK9" s="38" t="s">
         <v>29</v>
@@ -2550,6 +2584,17 @@
       <c r="AM9" s="8"/>
     </row>
     <row r="10" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="25"/>
+      <c r="D10" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5"/>
       <c r="K10" s="25"/>
       <c r="L10" s="19" t="s">
         <v>25</v>
@@ -2572,11 +2617,11 @@
         <v>39</v>
       </c>
       <c r="W10" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AI10" s="4"/>
       <c r="AJ10" s="18" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="AK10" s="18" t="s">
         <v>33</v>
@@ -2587,6 +2632,17 @@
       <c r="AM10" s="5"/>
     </row>
     <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C11" s="25"/>
+      <c r="D11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="K11" s="25"/>
       <c r="L11" s="19" t="s">
         <v>0</v>
@@ -2599,16 +2655,16 @@
       </c>
       <c r="O11" s="5"/>
       <c r="S11" s="23"/>
-      <c r="AA11" s="154" t="s">
+      <c r="AA11" s="126" t="s">
         <v>43</v>
       </c>
-      <c r="AB11" s="155"/>
-      <c r="AC11" s="155"/>
-      <c r="AD11" s="155"/>
-      <c r="AE11" s="156"/>
+      <c r="AB11" s="127"/>
+      <c r="AC11" s="127"/>
+      <c r="AD11" s="127"/>
+      <c r="AE11" s="128"/>
       <c r="AI11" s="4"/>
       <c r="AJ11" s="19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="AK11" s="64" t="s">
         <v>33</v>
@@ -2619,6 +2675,17 @@
       <c r="AM11" s="5"/>
     </row>
     <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C12" s="25"/>
+      <c r="D12" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="5"/>
       <c r="K12" s="25"/>
       <c r="L12" s="19" t="s">
         <v>26</v>
@@ -2651,7 +2718,7 @@
         <v>1</v>
       </c>
       <c r="AK12" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AL12" s="19" t="s">
         <v>39</v>
@@ -2659,6 +2726,17 @@
       <c r="AM12" s="5"/>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C13" s="25"/>
+      <c r="D13" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="K13" s="25"/>
       <c r="L13" s="19" t="s">
         <v>27</v>
@@ -2686,7 +2764,7 @@
       <c r="AE13" s="3"/>
       <c r="AI13" s="4"/>
       <c r="AJ13" s="18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="AK13" s="18" t="s">
         <v>33</v>
@@ -2697,6 +2775,17 @@
       <c r="AM13" s="5"/>
     </row>
     <row r="14" spans="1:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="25"/>
+      <c r="D14" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="K14" s="25"/>
       <c r="L14" s="19" t="s">
         <v>14</v>
@@ -2735,6 +2824,17 @@
       <c r="AM14" s="5"/>
     </row>
     <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C15" s="25"/>
+      <c r="D15" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E15" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="K15" s="37" t="s">
         <v>46</v>
       </c>
@@ -2748,13 +2848,13 @@
         <v>39</v>
       </c>
       <c r="O15" s="8"/>
-      <c r="S15" s="143" t="s">
+      <c r="S15" s="123" t="s">
         <v>37</v>
       </c>
-      <c r="T15" s="144"/>
-      <c r="U15" s="144"/>
-      <c r="V15" s="144"/>
-      <c r="W15" s="146"/>
+      <c r="T15" s="124"/>
+      <c r="U15" s="124"/>
+      <c r="V15" s="124"/>
+      <c r="W15" s="125"/>
       <c r="AA15" s="44" t="s">
         <v>46</v>
       </c>
@@ -2779,6 +2879,17 @@
       <c r="AM15" s="5"/>
     </row>
     <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="C16" s="25"/>
+      <c r="D16" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="5"/>
       <c r="K16" s="25"/>
       <c r="L16" s="19" t="s">
         <v>4</v>
@@ -2829,6 +2940,15 @@
       <c r="AM16" s="5"/>
     </row>
     <row r="17" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C17" s="25"/>
+      <c r="D17" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="5"/>
       <c r="K17" s="25"/>
       <c r="L17" s="19" t="s">
         <v>8</v>
@@ -2871,6 +2991,15 @@
       <c r="AM17" s="5"/>
     </row>
     <row r="18" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C18" s="25"/>
+      <c r="D18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="5"/>
       <c r="K18" s="25"/>
       <c r="L18" s="19" t="s">
         <v>5</v>
@@ -2917,10 +3046,19 @@
         <v>39</v>
       </c>
       <c r="AM18" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="25"/>
+      <c r="D19" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="18"/>
+      <c r="G19" s="5"/>
       <c r="K19" s="25"/>
       <c r="L19" s="19" t="s">
         <v>6</v>
@@ -2952,6 +3090,17 @@
       <c r="AE19" s="6"/>
     </row>
     <row r="20" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="25"/>
+      <c r="D20" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20" s="5"/>
       <c r="K20" s="26"/>
       <c r="L20" s="21" t="s">
         <v>3</v>
@@ -2963,7 +3112,7 @@
         <v>39</v>
       </c>
       <c r="O20" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S20" s="26"/>
       <c r="T20" s="21" t="s">
@@ -2976,19 +3125,41 @@
         <v>39</v>
       </c>
       <c r="W20" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="AI21" s="125" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ21" s="126"/>
-      <c r="AK21" s="126"/>
-      <c r="AL21" s="126"/>
-      <c r="AM21" s="127"/>
-    </row>
-    <row r="22" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C21" s="25"/>
+      <c r="D21" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="5"/>
+      <c r="AI21" s="138" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ21" s="139"/>
+      <c r="AK21" s="139"/>
+      <c r="AL21" s="139"/>
+      <c r="AM21" s="140"/>
+    </row>
+    <row r="22" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C22" s="26"/>
+      <c r="D22" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="AI22" s="104" t="s">
         <v>22</v>
       </c>
@@ -3006,11 +3177,12 @@
       </c>
     </row>
     <row r="23" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C23" s="23"/>
       <c r="AI23" s="107" t="s">
         <v>23</v>
       </c>
       <c r="AJ23" s="108" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="AK23" s="108" t="s">
         <v>29</v>
@@ -3046,34 +3218,41 @@
       </c>
       <c r="AM25" s="5"/>
     </row>
-    <row r="26" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="K26" s="147" t="s">
+    <row r="26" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K26" s="129" t="s">
         <v>50</v>
       </c>
-      <c r="L26" s="148"/>
-      <c r="M26" s="148"/>
-      <c r="N26" s="148"/>
-      <c r="O26" s="149"/>
-      <c r="S26" s="131" t="s">
-        <v>75</v>
-      </c>
-      <c r="T26" s="132"/>
-      <c r="U26" s="132"/>
-      <c r="V26" s="132"/>
-      <c r="W26" s="133"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="130"/>
+      <c r="N26" s="130"/>
+      <c r="O26" s="131"/>
+      <c r="S26" s="141" t="s">
+        <v>74</v>
+      </c>
+      <c r="T26" s="142"/>
+      <c r="U26" s="142"/>
+      <c r="V26" s="142"/>
+      <c r="W26" s="143"/>
       <c r="AI26" s="4"/>
       <c r="AJ26" s="18" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="AK26" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="AL26" s="18" t="s">
         <v>39</v>
       </c>
       <c r="AM26" s="5"/>
     </row>
-    <row r="27" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C27" s="154" t="s">
+        <v>141</v>
+      </c>
+      <c r="D27" s="155"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="156"/>
       <c r="K27" s="59" t="s">
         <v>22</v>
       </c>
@@ -3117,13 +3296,21 @@
       <c r="AM27" s="5"/>
     </row>
     <row r="28" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C28" s="143" t="s">
-        <v>60</v>
-      </c>
-      <c r="D28" s="144"/>
-      <c r="E28" s="144"/>
-      <c r="F28" s="145"/>
-      <c r="G28" s="146"/>
+      <c r="C28" s="53" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="E28" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="55" t="s">
+        <v>21</v>
+      </c>
       <c r="K28" s="62" t="s">
         <v>23</v>
       </c>
@@ -3141,7 +3328,7 @@
         <v>23</v>
       </c>
       <c r="T28" s="74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="U28" s="74" t="s">
         <v>29</v>
@@ -3161,21 +3348,19 @@
       <c r="AM28" s="5"/>
     </row>
     <row r="29" spans="3:39" x14ac:dyDescent="0.2">
-      <c r="C29" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E29" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="G29" s="43" t="s">
-        <v>21</v>
-      </c>
+      <c r="C29" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="58"/>
       <c r="K29" s="25"/>
       <c r="L29" s="19" t="s">
         <v>0</v>
@@ -3191,7 +3376,7 @@
         <v>46</v>
       </c>
       <c r="T29" s="63" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U29" s="63" t="s">
         <v>29</v>
@@ -3211,19 +3396,19 @@
       <c r="AM29" s="5"/>
     </row>
     <row r="30" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C30" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E30" s="45" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="7"/>
+      <c r="C30" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="63" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="10"/>
       <c r="K30" s="25"/>
       <c r="L30" s="19" t="s">
         <v>26</v>
@@ -3237,7 +3422,7 @@
       <c r="O30" s="5"/>
       <c r="S30" s="25"/>
       <c r="T30" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U30" s="18" t="s">
         <v>30</v>
@@ -3259,7 +3444,7 @@
         <v>39</v>
       </c>
       <c r="AM30" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="3:39" x14ac:dyDescent="0.2">
@@ -3268,14 +3453,12 @@
         <v>0</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F31" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="5"/>
       <c r="K31" s="25"/>
       <c r="L31" s="19" t="s">
         <v>27</v>
@@ -3287,30 +3470,28 @@
       <c r="O31" s="5"/>
       <c r="S31" s="25"/>
       <c r="T31" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="U31" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V31" s="18" t="s">
         <v>39</v>
       </c>
       <c r="W31" s="5"/>
     </row>
-    <row r="32" spans="3:39" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C32" s="26"/>
-      <c r="D32" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>63</v>
-      </c>
+    <row r="32" spans="3:39" x14ac:dyDescent="0.2">
+      <c r="C32" s="25"/>
+      <c r="D32" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G32" s="5"/>
       <c r="K32" s="25"/>
       <c r="L32" s="19" t="s">
         <v>14</v>
@@ -3324,10 +3505,10 @@
       <c r="O32" s="5"/>
       <c r="S32" s="25"/>
       <c r="T32" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="U32" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V32" s="18" t="s">
         <v>39</v>
@@ -3335,6 +3516,17 @@
       <c r="W32" s="5"/>
     </row>
     <row r="33" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C33" s="25"/>
+      <c r="D33" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G33" s="5"/>
       <c r="K33" s="25"/>
       <c r="L33" s="19" t="s">
         <v>25</v>
@@ -3348,23 +3540,34 @@
       <c r="O33" s="5"/>
       <c r="S33" s="25"/>
       <c r="T33" s="18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U33" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V33" s="18" t="s">
         <v>39</v>
       </c>
       <c r="W33" s="5"/>
     </row>
-    <row r="34" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C34" s="25"/>
+      <c r="D34" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="5"/>
       <c r="K34" s="25"/>
       <c r="L34" s="19" t="s">
         <v>12</v>
       </c>
       <c r="M34" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N34" s="19" t="s">
         <v>39</v>
@@ -3372,24 +3575,28 @@
       <c r="O34" s="5"/>
       <c r="S34" s="25"/>
       <c r="T34" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="U34" s="64" t="s">
         <v>41</v>
       </c>
       <c r="V34" s="18"/>
       <c r="W34" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="134" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="135"/>
-      <c r="E35" s="135"/>
-      <c r="F35" s="135"/>
-      <c r="G35" s="136"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G35" s="5"/>
       <c r="K35" s="25"/>
       <c r="L35" s="19" t="s">
         <v>52</v>
@@ -3405,7 +3612,7 @@
         <v>46</v>
       </c>
       <c r="T35" s="78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="U35" s="78" t="s">
         <v>29</v>
@@ -3416,26 +3623,22 @@
       <c r="W35" s="86"/>
     </row>
     <row r="36" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C36" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F36" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>21</v>
-      </c>
+      <c r="C36" s="25"/>
+      <c r="D36" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="5"/>
       <c r="K36" s="44" t="s">
         <v>46</v>
       </c>
       <c r="L36" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M36" s="66" t="s">
         <v>29</v>
@@ -3448,7 +3651,7 @@
         <v>46</v>
       </c>
       <c r="T36" s="99" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="U36" s="99" t="s">
         <v>29</v>
@@ -3457,33 +3660,31 @@
         <v>39</v>
       </c>
       <c r="W36" s="11"/>
-      <c r="AA36" s="125" t="s">
-        <v>112</v>
-      </c>
-      <c r="AB36" s="126"/>
-      <c r="AC36" s="126"/>
-      <c r="AD36" s="126"/>
-      <c r="AE36" s="127"/>
+      <c r="AA36" s="138" t="s">
+        <v>109</v>
+      </c>
+      <c r="AB36" s="139"/>
+      <c r="AC36" s="139"/>
+      <c r="AD36" s="139"/>
+      <c r="AE36" s="140"/>
     </row>
     <row r="37" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C37" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="G37" s="13"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E37" s="64" t="s">
+        <v>33</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G37" s="5"/>
       <c r="K37" s="24" t="s">
         <v>46</v>
       </c>
       <c r="L37" s="17" t="s">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="M37" s="17" t="s">
         <v>29</v>
@@ -3498,7 +3699,7 @@
         <v>46</v>
       </c>
       <c r="T37" s="57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="U37" s="57" t="s">
         <v>29</v>
@@ -3523,24 +3724,22 @@
     </row>
     <row r="38" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C38" s="25"/>
-      <c r="D38" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>73</v>
-      </c>
+      <c r="D38" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="5"/>
       <c r="K38" s="68"/>
       <c r="L38" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M38" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N38" s="19" t="s">
         <v>39</v>
@@ -3548,7 +3747,7 @@
       <c r="O38" s="9"/>
       <c r="S38" s="4"/>
       <c r="T38" s="18" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="U38" s="64" t="s">
         <v>41</v>
@@ -3559,7 +3758,7 @@
         <v>23</v>
       </c>
       <c r="AB38" s="108" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="AC38" s="108" t="s">
         <v>29</v>
@@ -3569,25 +3768,23 @@
       </c>
       <c r="AE38" s="109"/>
     </row>
-    <row r="39" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C39" s="26"/>
-      <c r="D39" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F39" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>63</v>
-      </c>
+    <row r="39" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C39" s="25"/>
+      <c r="D39" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G39" s="5"/>
       <c r="K39" s="73" t="s">
         <v>46</v>
       </c>
       <c r="L39" s="74" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M39" s="74" t="s">
         <v>29</v>
@@ -3598,7 +3795,7 @@
       <c r="O39" s="75"/>
       <c r="S39" s="68"/>
       <c r="T39" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="U39" s="18" t="s">
         <v>30</v>
@@ -3609,7 +3806,7 @@
         <v>46</v>
       </c>
       <c r="AB39" s="74" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="AC39" s="74" t="s">
         <v>29</v>
@@ -3620,6 +3817,17 @@
       <c r="AE39" s="75"/>
     </row>
     <row r="40" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C40" s="25"/>
+      <c r="D40" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="5"/>
       <c r="K40" s="76" t="s">
         <v>46</v>
       </c>
@@ -3646,7 +3854,7 @@
         <v>46</v>
       </c>
       <c r="AB40" s="91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC40" s="91" t="s">
         <v>29</v>
@@ -3657,19 +3865,28 @@
       <c r="AE40" s="14"/>
     </row>
     <row r="41" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K41" s="98" t="s">
-        <v>46</v>
-      </c>
-      <c r="L41" s="99" t="s">
-        <v>85</v>
-      </c>
-      <c r="M41" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="N41" s="99" t="s">
-        <v>39</v>
-      </c>
-      <c r="O41" s="11"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="64" t="s">
+        <v>41</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N41" s="19"/>
+      <c r="O41" s="5" t="s">
+        <v>73</v>
+      </c>
       <c r="S41" s="26"/>
       <c r="T41" s="21" t="s">
         <v>6</v>
@@ -3681,7 +3898,7 @@
       <c r="W41" s="6"/>
       <c r="AA41" s="20"/>
       <c r="AB41" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AC41" s="22" t="s">
         <v>29</v>
@@ -3692,161 +3909,116 @@
       <c r="AE41" s="6"/>
     </row>
     <row r="42" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C42" s="131" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42" s="132"/>
-      <c r="E42" s="132"/>
-      <c r="F42" s="132"/>
-      <c r="G42" s="133"/>
-      <c r="K42" s="56" t="s">
-        <v>46</v>
-      </c>
-      <c r="L42" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="M42" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="N42" s="57"/>
-      <c r="O42" s="58"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F42" s="19"/>
+      <c r="G42" s="5"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="M42" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="N42" s="18"/>
+      <c r="O42" s="5"/>
     </row>
     <row r="43" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C43" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="70" t="s">
-        <v>19</v>
-      </c>
-      <c r="E43" s="70" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="71" t="s">
-        <v>40</v>
-      </c>
-      <c r="G43" s="72" t="s">
-        <v>21</v>
-      </c>
+      <c r="C43" s="25"/>
+      <c r="D43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="18"/>
+      <c r="G43" s="5"/>
       <c r="K43" s="25"/>
       <c r="L43" s="19" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M43" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="N43" s="19"/>
-      <c r="O43" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="N43" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="O43" s="5"/>
     </row>
     <row r="44" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C44" s="73" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="74" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="F44" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="G44" s="75"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E44" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G44" s="5"/>
       <c r="K44" s="25"/>
       <c r="L44" s="19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="M44" s="18" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N44" s="18"/>
       <c r="O44" s="5"/>
     </row>
     <row r="45" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C45" s="25"/>
-      <c r="D45" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F45" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K45" s="25"/>
-      <c r="L45" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="M45" s="18" t="s">
+      <c r="D45" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="N45" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="O45" s="5"/>
-    </row>
-    <row r="46" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C46" s="4"/>
-      <c r="D46" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F46" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="K46" s="25"/>
-      <c r="L46" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="M46" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="N46" s="18"/>
-      <c r="O46" s="5"/>
-      <c r="S46" s="137" t="s">
-        <v>87</v>
-      </c>
-      <c r="T46" s="138"/>
-      <c r="U46" s="138"/>
-      <c r="V46" s="138"/>
-      <c r="W46" s="139"/>
-    </row>
-    <row r="47" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C47" s="26"/>
-      <c r="D47" s="21" t="s">
+      <c r="F45" s="18"/>
+      <c r="G45" s="5"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E47" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K47" s="26"/>
-      <c r="L47" s="21" t="s">
+      <c r="M45" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N45" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="46" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C46" s="26"/>
+      <c r="D46" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="M47" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N47" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="O47" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="E46" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="S46" s="147" t="s">
+        <v>86</v>
+      </c>
+      <c r="T46" s="148"/>
+      <c r="U46" s="148"/>
+      <c r="V46" s="148"/>
+      <c r="W46" s="149"/>
+    </row>
+    <row r="47" spans="3:31" x14ac:dyDescent="0.2">
       <c r="S47" s="87" t="s">
         <v>22</v>
       </c>
@@ -3875,7 +4047,7 @@
         <v>23</v>
       </c>
       <c r="T48" s="91" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U48" s="91" t="s">
         <v>29</v>
@@ -3905,56 +4077,41 @@
       </c>
       <c r="W49" s="5"/>
     </row>
-    <row r="50" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C50" s="116" t="s">
-        <v>68</v>
-      </c>
-      <c r="D50" s="117"/>
-      <c r="E50" s="117"/>
-      <c r="F50" s="117"/>
-      <c r="G50" s="118"/>
-      <c r="K50" s="116" t="s">
-        <v>105</v>
-      </c>
-      <c r="L50" s="117"/>
-      <c r="M50" s="117"/>
-      <c r="N50" s="117"/>
-      <c r="O50" s="118"/>
+    <row r="50" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K50" s="132" t="s">
+        <v>103</v>
+      </c>
+      <c r="L50" s="133"/>
+      <c r="M50" s="133"/>
+      <c r="N50" s="133"/>
+      <c r="O50" s="134"/>
       <c r="S50" s="25"/>
       <c r="T50" s="18" t="s">
         <v>1</v>
       </c>
       <c r="U50" s="18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="V50" s="18" t="s">
         <v>39</v>
       </c>
       <c r="W50" s="5"/>
-      <c r="AA50" s="140" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB50" s="141"/>
-      <c r="AC50" s="141"/>
-      <c r="AD50" s="141"/>
-      <c r="AE50" s="142"/>
+      <c r="AA50" s="150" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB50" s="151"/>
+      <c r="AC50" s="151"/>
+      <c r="AD50" s="151"/>
+      <c r="AE50" s="152"/>
     </row>
     <row r="51" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C51" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="81" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="82" t="s">
-        <v>40</v>
-      </c>
-      <c r="G51" s="83" t="s">
-        <v>21</v>
-      </c>
+      <c r="C51" s="123" t="s">
+        <v>59</v>
+      </c>
+      <c r="D51" s="124"/>
+      <c r="E51" s="124"/>
+      <c r="F51" s="153"/>
+      <c r="G51" s="125"/>
       <c r="K51" s="80" t="s">
         <v>22</v>
       </c>
@@ -3972,10 +4129,10 @@
       </c>
       <c r="S51" s="25"/>
       <c r="T51" s="18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U51" s="18" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V51" s="18" t="s">
         <v>39</v>
@@ -3998,24 +4155,26 @@
       </c>
     </row>
     <row r="52" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C52" s="84" t="s">
-        <v>23</v>
-      </c>
-      <c r="D52" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="F52" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="G52" s="86"/>
+      <c r="C52" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" s="43" t="s">
+        <v>21</v>
+      </c>
       <c r="K52" s="84" t="s">
         <v>23</v>
       </c>
       <c r="L52" s="78" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M52" s="78" t="s">
         <v>29</v>
@@ -4026,7 +4185,7 @@
       <c r="O52" s="86"/>
       <c r="S52" s="25"/>
       <c r="T52" s="19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="U52" s="18" t="s">
         <v>33</v>
@@ -4039,7 +4198,7 @@
         <v>23</v>
       </c>
       <c r="AB52" s="96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AC52" s="96" t="s">
         <v>29</v>
@@ -4050,19 +4209,19 @@
       <c r="AE52" s="16"/>
     </row>
     <row r="53" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C53" s="25"/>
-      <c r="D53" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="F53" s="31" t="s">
-        <v>39</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>69</v>
-      </c>
+      <c r="C53" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D53" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E53" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="46" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="7"/>
       <c r="K53" s="25"/>
       <c r="L53" s="18" t="s">
         <v>0</v>
@@ -4074,11 +4233,11 @@
         <v>39</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S53" s="25"/>
       <c r="T53" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="U53" s="18" t="s">
         <v>33</v>
@@ -4091,7 +4250,7 @@
         <v>46</v>
       </c>
       <c r="AB53" s="91" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AC53" s="91" t="s">
         <v>29</v>
@@ -4102,18 +4261,18 @@
       <c r="AE53" s="14"/>
     </row>
     <row r="54" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C54" s="26"/>
-      <c r="D54" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F54" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>63</v>
+      <c r="C54" s="25"/>
+      <c r="D54" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="K54" s="26"/>
       <c r="L54" s="21" t="s">
@@ -4126,11 +4285,11 @@
         <v>39</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S54" s="25"/>
       <c r="T54" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="U54" s="18" t="s">
         <v>29</v>
@@ -4144,17 +4303,30 @@
         <v>0</v>
       </c>
       <c r="AC54" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD54" s="19" t="s">
         <v>39</v>
       </c>
       <c r="AE54" s="5"/>
     </row>
-    <row r="55" spans="3:31" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="26"/>
+      <c r="D55" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F55" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="S55" s="4"/>
       <c r="T55" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="U55" s="18" t="s">
         <v>33</v>
@@ -4163,7 +4335,7 @@
         <v>39</v>
       </c>
       <c r="W55" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="AA55" s="25"/>
       <c r="AB55" s="18" t="s">
@@ -4177,10 +4349,10 @@
       </c>
       <c r="AE55" s="5"/>
     </row>
-    <row r="56" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:31" x14ac:dyDescent="0.2">
       <c r="S56" s="4"/>
       <c r="T56" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="U56" s="18" t="s">
         <v>31</v>
@@ -4203,19 +4375,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C57" s="119" t="s">
-        <v>96</v>
-      </c>
-      <c r="D57" s="120"/>
-      <c r="E57" s="120"/>
-      <c r="F57" s="120"/>
-      <c r="G57" s="121"/>
+    <row r="57" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="S57" s="62" t="s">
         <v>46</v>
       </c>
       <c r="T57" s="63" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="U57" s="63" t="s">
         <v>29</v>
@@ -4226,7 +4391,7 @@
       <c r="W57" s="10"/>
       <c r="AA57" s="4"/>
       <c r="AB57" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="AC57" s="64" t="s">
         <v>33</v>
@@ -4237,21 +4402,13 @@
       <c r="AE57" s="5"/>
     </row>
     <row r="58" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C58" s="100" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="101" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" s="101" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="101" t="s">
-        <v>40</v>
-      </c>
-      <c r="G58" s="102" t="s">
-        <v>21</v>
-      </c>
+      <c r="C58" s="144" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="145"/>
+      <c r="E58" s="145"/>
+      <c r="F58" s="145"/>
+      <c r="G58" s="146"/>
       <c r="S58" s="4"/>
       <c r="T58" s="19" t="s">
         <v>2</v>
@@ -4276,19 +4433,21 @@
       <c r="AE58" s="5"/>
     </row>
     <row r="59" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="98" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="99" t="s">
-        <v>97</v>
-      </c>
-      <c r="E59" s="99" t="s">
-        <v>29</v>
-      </c>
-      <c r="F59" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="G59" s="11"/>
+      <c r="C59" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="G59" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="S59" s="26"/>
       <c r="T59" s="21" t="s">
         <v>3</v>
@@ -4300,7 +4459,7 @@
         <v>39</v>
       </c>
       <c r="W59" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA59" s="25"/>
       <c r="AB59" s="19" t="s">
@@ -4317,19 +4476,21 @@
       </c>
     </row>
     <row r="60" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C60" s="4"/>
-      <c r="D60" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G60" s="5"/>
+      <c r="C60" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="E60" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F60" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="13"/>
       <c r="T60" s="111" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AA60" s="25"/>
       <c r="AB60" s="19" t="s">
@@ -4344,17 +4505,19 @@
       </c>
     </row>
     <row r="61" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C61" s="4"/>
+      <c r="C61" s="25"/>
       <c r="D61" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E61" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G61" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F61" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="AA61" s="25"/>
       <c r="AB61" s="19" t="s">
         <v>5</v>
@@ -4367,18 +4530,20 @@
       </c>
       <c r="AE61" s="5"/>
     </row>
-    <row r="62" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C62" s="4"/>
-      <c r="D62" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E62" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F62" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G62" s="5"/>
+    <row r="62" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="26"/>
+      <c r="D62" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F62" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="AA62" s="25"/>
       <c r="AB62" s="19" t="s">
         <v>6</v>
@@ -4390,17 +4555,6 @@
       <c r="AE62" s="5"/>
     </row>
     <row r="63" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C63" s="4"/>
-      <c r="D63" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E63" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G63" s="5"/>
       <c r="AA63" s="26"/>
       <c r="AB63" s="22" t="s">
         <v>3</v>
@@ -4410,67 +4564,57 @@
       </c>
       <c r="AD63" s="22"/>
       <c r="AE63" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="141" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="64" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C64" s="4"/>
-      <c r="D64" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E64" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G64" s="5"/>
-    </row>
-    <row r="65" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="4"/>
-      <c r="D65" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E65" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G65" s="5"/>
+      <c r="D65" s="142"/>
+      <c r="E65" s="142"/>
+      <c r="F65" s="142"/>
+      <c r="G65" s="143"/>
     </row>
     <row r="66" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C66" s="4"/>
-      <c r="D66" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E66" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G66" s="5"/>
-      <c r="AA66" s="147" t="s">
-        <v>134</v>
-      </c>
-      <c r="AB66" s="148"/>
-      <c r="AC66" s="148"/>
-      <c r="AD66" s="148"/>
-      <c r="AE66" s="149"/>
+      <c r="C66" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="70" t="s">
+        <v>19</v>
+      </c>
+      <c r="E66" s="70" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="72" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA66" s="129" t="s">
+        <v>131</v>
+      </c>
+      <c r="AB66" s="130"/>
+      <c r="AC66" s="130"/>
+      <c r="AD66" s="130"/>
+      <c r="AE66" s="131"/>
     </row>
     <row r="67" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="4"/>
-      <c r="D67" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E67" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G67" s="5"/>
+      <c r="C67" s="73" t="s">
+        <v>23</v>
+      </c>
+      <c r="D67" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="E67" s="74" t="s">
+        <v>29</v>
+      </c>
+      <c r="F67" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="75"/>
       <c r="AA67" s="59" t="s">
         <v>22</v>
       </c>
@@ -4488,29 +4632,31 @@
       </c>
     </row>
     <row r="68" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C68" s="4"/>
-      <c r="D68" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E68" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G68" s="5"/>
-      <c r="S68" s="125" t="s">
-        <v>130</v>
-      </c>
-      <c r="T68" s="126"/>
-      <c r="U68" s="126"/>
-      <c r="V68" s="126"/>
-      <c r="W68" s="127"/>
+      <c r="C68" s="25"/>
+      <c r="D68" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F68" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="S68" s="138" t="s">
+        <v>127</v>
+      </c>
+      <c r="T68" s="139"/>
+      <c r="U68" s="139"/>
+      <c r="V68" s="139"/>
+      <c r="W68" s="140"/>
       <c r="AA68" s="62" t="s">
         <v>23</v>
       </c>
       <c r="AB68" s="63" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="AC68" s="63" t="s">
         <v>29</v>
@@ -4522,16 +4668,18 @@
     </row>
     <row r="69" spans="3:31" x14ac:dyDescent="0.2">
       <c r="C69" s="4"/>
-      <c r="D69" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E69" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G69" s="5"/>
+      <c r="D69" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F69" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>134</v>
+      </c>
       <c r="S69" s="104" t="s">
         <v>22</v>
       </c>
@@ -4552,7 +4700,7 @@
         <v>0</v>
       </c>
       <c r="AC69" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD69" s="19" t="s">
         <v>39</v>
@@ -4560,20 +4708,24 @@
       <c r="AE69" s="5"/>
     </row>
     <row r="70" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C70" s="4"/>
-      <c r="D70" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F70" s="18"/>
-      <c r="G70" s="5"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F70" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="S70" s="112" t="s">
         <v>23</v>
       </c>
       <c r="T70" s="113" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="U70" s="113" t="s">
         <v>29</v>
@@ -4593,76 +4745,57 @@
         <v>39</v>
       </c>
       <c r="AE70" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="71" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C71" s="4"/>
-      <c r="D71" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F71" s="19"/>
-      <c r="G71" s="5"/>
-    </row>
-    <row r="72" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C72" s="4"/>
-      <c r="D72" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E72" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F72" s="18"/>
-      <c r="G72" s="5"/>
-    </row>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="72" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="4"/>
-      <c r="D73" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E73" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G73" s="5"/>
+      <c r="C73" s="132" t="s">
+        <v>67</v>
+      </c>
+      <c r="D73" s="133"/>
+      <c r="E73" s="133"/>
+      <c r="F73" s="133"/>
+      <c r="G73" s="134"/>
     </row>
     <row r="74" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C74" s="4"/>
-      <c r="D74" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F74" s="18"/>
-      <c r="G74" s="5"/>
-      <c r="S74" s="131" t="s">
-        <v>127</v>
-      </c>
-      <c r="T74" s="132"/>
-      <c r="U74" s="132"/>
-      <c r="V74" s="132"/>
-      <c r="W74" s="133"/>
-    </row>
-    <row r="75" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C75" s="20"/>
-      <c r="D75" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E75" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F75" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G75" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="C74" s="80" t="s">
+        <v>22</v>
+      </c>
+      <c r="D74" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="E74" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="F74" s="82" t="s">
+        <v>40</v>
+      </c>
+      <c r="G74" s="83" t="s">
+        <v>21</v>
+      </c>
+      <c r="S74" s="141" t="s">
+        <v>124</v>
+      </c>
+      <c r="T74" s="142"/>
+      <c r="U74" s="142"/>
+      <c r="V74" s="142"/>
+      <c r="W74" s="143"/>
+    </row>
+    <row r="75" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C75" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="D75" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" s="85" t="s">
+        <v>34</v>
+      </c>
+      <c r="G75" s="86"/>
       <c r="S75" s="69" t="s">
         <v>22</v>
       </c>
@@ -4680,11 +4813,24 @@
       </c>
     </row>
     <row r="76" spans="3:31" x14ac:dyDescent="0.2">
+      <c r="C76" s="25"/>
+      <c r="D76" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F76" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="G76" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="S76" s="73" t="s">
         <v>23</v>
       </c>
       <c r="T76" s="74" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="U76" s="74" t="s">
         <v>29</v>
@@ -4695,11 +4841,24 @@
       <c r="W76" s="75"/>
     </row>
     <row r="77" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="26"/>
+      <c r="D77" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="F77" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="S77" s="25" t="s">
         <v>46</v>
       </c>
       <c r="T77" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="U77" s="18" t="s">
         <v>29</v>
@@ -4710,16 +4869,9 @@
       <c r="W77" s="5"/>
     </row>
     <row r="78" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C78" s="122" t="s">
-        <v>107</v>
-      </c>
-      <c r="D78" s="123"/>
-      <c r="E78" s="123"/>
-      <c r="F78" s="123"/>
-      <c r="G78" s="124"/>
       <c r="S78" s="4"/>
       <c r="T78" s="18" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="U78" s="18" t="s">
         <v>29</v>
@@ -4730,24 +4882,9 @@
       <c r="W78" s="5"/>
     </row>
     <row r="79" spans="3:31" x14ac:dyDescent="0.2">
-      <c r="C79" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="D79" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E79" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G79" s="55" t="s">
-        <v>21</v>
-      </c>
       <c r="S79" s="4"/>
       <c r="T79" s="18" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="U79" s="18" t="s">
         <v>29</v>
@@ -4758,19 +4895,6 @@
       <c r="W79" s="5"/>
     </row>
     <row r="80" spans="3:31" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="D80" s="57" t="s">
-        <v>108</v>
-      </c>
-      <c r="E80" s="57" t="s">
-        <v>29</v>
-      </c>
-      <c r="F80" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="G80" s="58"/>
       <c r="S80" s="20"/>
       <c r="T80" s="22" t="s">
         <v>3</v>
@@ -4782,239 +4906,37 @@
         <v>39</v>
       </c>
       <c r="W80" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="81" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C81" s="4"/>
-      <c r="D81" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G81" s="5"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="81" spans="20:20" x14ac:dyDescent="0.2">
       <c r="T81" s="111" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="82" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C82" s="4"/>
-      <c r="D82" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G82" s="5"/>
-    </row>
-    <row r="83" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C83" s="4"/>
-      <c r="D83" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="E83" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F83" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G83" s="5"/>
-    </row>
-    <row r="84" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C84" s="4"/>
-      <c r="D84" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F84" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G84" s="5"/>
-    </row>
-    <row r="85" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C85" s="4"/>
-      <c r="D85" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E85" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F85" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G85" s="5"/>
-    </row>
-    <row r="86" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C86" s="4"/>
-      <c r="D86" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E86" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="F86" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G86" s="5"/>
-    </row>
-    <row r="87" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C87" s="4"/>
-      <c r="D87" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E87" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="F87" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G87" s="5"/>
-    </row>
-    <row r="88" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C88" s="4"/>
-      <c r="D88" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="E88" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F88" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G88" s="5"/>
-    </row>
-    <row r="89" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C89" s="4"/>
-      <c r="D89" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="E89" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F89" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G89" s="5"/>
-    </row>
-    <row r="90" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C90" s="4"/>
-      <c r="D90" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E90" s="64" t="s">
-        <v>109</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G90" s="5"/>
-    </row>
-    <row r="91" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C91" s="4"/>
-      <c r="D91" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E91" s="64" t="s">
-        <v>41</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C92" s="4"/>
-      <c r="D92" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="E92" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F92" s="19"/>
-      <c r="G92" s="5"/>
-    </row>
-    <row r="93" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C93" s="4"/>
-      <c r="D93" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F93" s="18"/>
-      <c r="G93" s="5"/>
-    </row>
-    <row r="94" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C94" s="4"/>
-      <c r="D94" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="E94" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F94" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G94" s="5"/>
-    </row>
-    <row r="95" spans="3:20" x14ac:dyDescent="0.2">
-      <c r="C95" s="4"/>
-      <c r="D95" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E95" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="F95" s="18"/>
-      <c r="G95" s="5"/>
-    </row>
-    <row r="96" spans="3:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C96" s="20"/>
-      <c r="D96" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="E96" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F96" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G96" s="6" t="s">
-        <v>63</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C27:G27"/>
+    <mergeCell ref="K50:O50"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="AA36:AE36"/>
+    <mergeCell ref="AI7:AM7"/>
+    <mergeCell ref="AI21:AM21"/>
+    <mergeCell ref="S74:W74"/>
+    <mergeCell ref="S68:W68"/>
+    <mergeCell ref="C65:G65"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="S26:W26"/>
+    <mergeCell ref="C73:G73"/>
+    <mergeCell ref="S46:W46"/>
+    <mergeCell ref="AA50:AE50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="AA66:AE66"/>
     <mergeCell ref="K6:O6"/>
     <mergeCell ref="S6:W6"/>
     <mergeCell ref="S15:W15"/>
     <mergeCell ref="AA11:AE11"/>
     <mergeCell ref="K26:O26"/>
-    <mergeCell ref="K50:O50"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C78:G78"/>
-    <mergeCell ref="AA36:AE36"/>
-    <mergeCell ref="AI7:AM7"/>
-    <mergeCell ref="AI21:AM21"/>
-    <mergeCell ref="S74:W74"/>
-    <mergeCell ref="S68:W68"/>
-    <mergeCell ref="C42:G42"/>
-    <mergeCell ref="C35:G35"/>
-    <mergeCell ref="S26:W26"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="S46:W46"/>
-    <mergeCell ref="AA50:AE50"/>
-    <mergeCell ref="C28:G28"/>
-    <mergeCell ref="AA66:AE66"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>